<commit_message>
Purchase Price List Mass Upload
</commit_message>
<xml_diff>
--- a/MassUpload/templates/Discount-Matrix-Template.xlsx
+++ b/MassUpload/templates/Discount-Matrix-Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\myxfin_st\MassUpload\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45211FDB-06B0-49EF-8CD3-B6F1DB22AD64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EFA498-DD5E-4ACC-A20D-F198E4182026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="975" windowWidth="20370" windowHeight="9825" xr2:uid="{BBB8F05F-B115-44FB-9F46-89E7969CBBE4}"/>
   </bookViews>
@@ -43,7 +43,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Item Number </t>
+      <t xml:space="preserve">Discount Price / Percentage </t>
     </r>
     <r>
       <rPr>
@@ -62,7 +62,7 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-(Name of the Discount)</t>
+(Accept Number/Decimal)</t>
     </r>
   </si>
   <si>
@@ -73,7 +73,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Unit </t>
+      <t xml:space="preserve">Item Number </t>
     </r>
     <r>
       <rPr>
@@ -92,7 +92,7 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-(Name of the Discount)</t>
+(Name of the Item)</t>
     </r>
   </si>
   <si>
@@ -103,7 +103,7 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve">Discount Price / Percentage </t>
+      <t xml:space="preserve">UOM / Unit </t>
     </r>
     <r>
       <rPr>
@@ -114,15 +114,6 @@
         <family val="2"/>
       </rPr>
       <t>*</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">
-(Accept Number/Decimal)</t>
     </r>
   </si>
   <si>
@@ -152,7 +143,7 @@
         <family val="2"/>
       </rPr>
       <t xml:space="preserve">
-(Enter if Price or PERCENT)</t>
+(Enter if PRICE or PERCENT Capitalize)</t>
     </r>
   </si>
 </sst>
@@ -210,7 +201,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -219,6 +210,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -538,7 +532,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,13 +545,13 @@
   <sheetData>
     <row r="1" spans="1:4" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
+      <c r="B1" s="6" t="s">
+        <v>2</v>
+      </c>
       <c r="C1" s="3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>3</v>

</xml_diff>